<commit_message>
Luân cung Điền Trạch)
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E35403-E9E8-4241-A920-FED681858900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FF6962-ABC1-466E-9BA1-60217D068BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7622" uniqueCount="3734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7696" uniqueCount="3770">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -11227,6 +11227,114 @@
   </si>
   <si>
     <t>Thai Phụ tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Tham Lang tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thất Sát tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Phá Quân tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Thiên Phủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Thiên Tướng tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Thất Sát tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Phá Quân tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Tham Lang tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung với Thiên Lương tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung với Cự Môn tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung với Phá Quân tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung với Thiên Phủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung với Thiên Tướng tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Thất Sát tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung với Cự Môn tại Điền Trạch ở Dần</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung với Cự Môn tại Điền Trạch ở Thân</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung với Thiên Lương tại Điền Trạch ở Mão</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung với Thiên Lương tại Điền Trạch ở Dậu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thiên Lương tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung với Cự Môn tại Điền Trạch ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung với Cự Môn tại Điền Trạch ở Dậu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung với Thái Âm tại Điền Trạch ở Dần</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung với Thái Âm tại Điền Trạch ở Thân</t>
+  </si>
+  <si>
+    <t>Thái Âm đồng cung Thiên Đồng tại Điền Trạch ở Ngọ</t>
+  </si>
+  <si>
+    <t>Kình Dương, Địa Không, Địa Kiếp đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cự Môn, Hỏa Tinh đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thái Âm, Đà La, Hóa Kỵ đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Hỏa Tinh đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Bạch Hổ, Kình Dương, Đà La đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh, Linh Tinh, Thiên Tướng, Phục Binh đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh, Tang Môn đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Địa Không, Địa Kiếp, Thiên Tướng, Phục Binh, Tả Phù, Hữu Bật đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Địa Không, Địa Kiếp, Thiên Tướng, Phục Binh, Kình Dương, Đà La đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Khốc, Thiên Hư đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Khốc, Thiên Hư, Hỏa Tinh, Linh Tinh, Tấu Thư đồng cung tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hồng Loan, Hoa Cái, Thiên Riêu đồng cung tại Điền Trạch</t>
   </si>
 </sst>
 </file>
@@ -11268,7 +11376,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11765,10 +11893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B3812"/>
+  <dimension ref="A1:B3850"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1640" workbookViewId="0">
-      <selection activeCell="J1670" sqref="J1670"/>
+    <sheetView tabSelected="1" topLeftCell="A3803" workbookViewId="0">
+      <selection activeCell="V3811" sqref="V3811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42264,55 +42392,355 @@
         <v>3612</v>
       </c>
     </row>
+    <row r="3814" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3814" t="s">
+        <v>3734</v>
+      </c>
+      <c r="B3814" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="3815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3815" t="s">
+        <v>3735</v>
+      </c>
+      <c r="B3815" t="s">
+        <v>3735</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3816" t="s">
+        <v>3736</v>
+      </c>
+      <c r="B3816" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3817" t="s">
+        <v>3737</v>
+      </c>
+      <c r="B3817" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="3818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3818" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B3818" t="s">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="3819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3819" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B3819" t="s">
+        <v>3739</v>
+      </c>
+    </row>
+    <row r="3820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3820" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B3820" t="s">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="3821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3821" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B3821" t="s">
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="3822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3822" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B3822" t="s">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="3823" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3823" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B3823" t="s">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="3824" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3824" t="s">
+        <v>3744</v>
+      </c>
+      <c r="B3824" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="3825" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3825" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B3825" t="s">
+        <v>3745</v>
+      </c>
+    </row>
+    <row r="3826" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3826" t="s">
+        <v>3746</v>
+      </c>
+      <c r="B3826" t="s">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="3827" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3827" t="s">
+        <v>3747</v>
+      </c>
+      <c r="B3827" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="3828" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3828" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3828" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3829" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3829" t="s">
+        <v>3748</v>
+      </c>
+      <c r="B3829" t="s">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="3830" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3830" t="s">
+        <v>3749</v>
+      </c>
+      <c r="B3830" t="s">
+        <v>3749</v>
+      </c>
+    </row>
+    <row r="3831" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3831" t="s">
+        <v>3750</v>
+      </c>
+      <c r="B3831" t="s">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="3832" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3832" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B3832" t="s">
+        <v>3751</v>
+      </c>
+    </row>
+    <row r="3833" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3833" t="s">
+        <v>3752</v>
+      </c>
+      <c r="B3833" t="s">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="3834" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3834" t="s">
+        <v>3753</v>
+      </c>
+      <c r="B3834" t="s">
+        <v>3753</v>
+      </c>
+    </row>
+    <row r="3835" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3835" t="s">
+        <v>3754</v>
+      </c>
+      <c r="B3835" t="s">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="3836" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3836" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B3836" t="s">
+        <v>3755</v>
+      </c>
+    </row>
+    <row r="3837" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3837" t="s">
+        <v>3756</v>
+      </c>
+      <c r="B3837" t="s">
+        <v>3756</v>
+      </c>
+    </row>
+    <row r="3838" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3838" t="s">
+        <v>3757</v>
+      </c>
+      <c r="B3838" t="s">
+        <v>3757</v>
+      </c>
+    </row>
+    <row r="3839" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3839" t="s">
+        <v>3758</v>
+      </c>
+      <c r="B3839" t="s">
+        <v>3758</v>
+      </c>
+    </row>
+    <row r="3840" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3840" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B3840" t="s">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="3841" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3841" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B3841" t="s">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="3842" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3842" t="s">
+        <v>3761</v>
+      </c>
+      <c r="B3842" t="s">
+        <v>3761</v>
+      </c>
+    </row>
+    <row r="3843" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3843" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B3843" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="3844" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3844" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B3844" t="s">
+        <v>3763</v>
+      </c>
+    </row>
+    <row r="3845" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3845" t="s">
+        <v>3764</v>
+      </c>
+      <c r="B3845" t="s">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="3846" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3846" t="s">
+        <v>3765</v>
+      </c>
+      <c r="B3846" t="s">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="3847" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3847" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B3847" t="s">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="3848" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3848" t="s">
+        <v>3767</v>
+      </c>
+      <c r="B3848" t="s">
+        <v>3767</v>
+      </c>
+    </row>
+    <row r="3849" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3849" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B3849" t="s">
+        <v>3768</v>
+      </c>
+    </row>
+    <row r="3850" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3850" t="s">
+        <v>3769</v>
+      </c>
+      <c r="B3850" t="s">
+        <v>3769</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="21" priority="68"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="19" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="17" priority="42"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="15" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="77"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="81"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="12" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209:B1631 B1:B23 B25:B84 B143">
-    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1805:B1809 B3442:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="19"/>
+  <conditionalFormatting sqref="B1805:B1809 B3442:B3813 B3851:B1048576">
+    <cfRule type="duplicateValues" dxfId="4" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1810:B3339">
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3814:B3850">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Hoàn Thiện luận 12 cung giừo chỉ thay giá trị trong excel
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC19BC16-5997-497A-938A-ED2E6C11511B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DC6215-C802-4633-84D5-38AF03D2592C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7750" uniqueCount="3797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7820" uniqueCount="3832">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -11416,6 +11416,111 @@
   </si>
   <si>
     <t>Hổ Tang Không Kiếp</t>
+  </si>
+  <si>
+    <t>Âm Dương Lương</t>
+  </si>
+  <si>
+    <t>Cơ Lương Gia Hội</t>
+  </si>
+  <si>
+    <t>Nhật Chiếu Lôi Môn</t>
+  </si>
+  <si>
+    <t>Tả Hữu Xương Khúc</t>
+  </si>
+  <si>
+    <t>Tham Linh Triều Viên</t>
+  </si>
+  <si>
+    <t>Cự Hỏa Linh</t>
+  </si>
+  <si>
+    <t>Hồng Đào Kỵ</t>
+  </si>
+  <si>
+    <t>Cự Đồng Hình</t>
+  </si>
+  <si>
+    <t>Lương Phá</t>
+  </si>
+  <si>
+    <t>Khôi Việt</t>
+  </si>
+  <si>
+    <t>Tham Vũ Hỏa</t>
+  </si>
+  <si>
+    <t>Cự Kỵ</t>
+  </si>
+  <si>
+    <t>Kình Đà Hỏa</t>
+  </si>
+  <si>
+    <t>Kình Đà Không Kiếp</t>
+  </si>
+  <si>
+    <t>Đào Hồng Hỷ</t>
+  </si>
+  <si>
+    <t>Đào Hồng Kiếp Sát</t>
+  </si>
+  <si>
+    <t>Đào Hồng Kỵ</t>
+  </si>
+  <si>
+    <t>Đào Hồng Tả Phù Hữu Bật</t>
+  </si>
+  <si>
+    <t>Đào Hồng Tả Phù Hữu Bật Khoa Quyền Lộc</t>
+  </si>
+  <si>
+    <t>Đào Hồng Tả Phù Hữu Bật Khoa Quyền Lộc Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Lưu Hà Kiếp Sát</t>
+  </si>
+  <si>
+    <t>Phục Không Kiếp</t>
+  </si>
+  <si>
+    <t>Xương Khúc Khôi Việt</t>
+  </si>
+  <si>
+    <t>Khoa Quyền</t>
+  </si>
+  <si>
+    <t>Lộc Quyền</t>
+  </si>
+  <si>
+    <t>Tướng Binh Đào Hồng</t>
+  </si>
+  <si>
+    <t>Lương Khốc Tuế</t>
+  </si>
+  <si>
+    <t>Tướng Binh</t>
+  </si>
+  <si>
+    <t>Cự Tang</t>
+  </si>
+  <si>
+    <t>Cự Hỏa</t>
+  </si>
+  <si>
+    <t>Phá Hình Kỵ</t>
+  </si>
+  <si>
+    <t>Tang Trực Tuế</t>
+  </si>
+  <si>
+    <t>Tuế Xương Khúc</t>
+  </si>
+  <si>
+    <t>Tử Vi Tả Hữu</t>
+  </si>
+  <si>
+    <t>Tử Vi Tang Tả Hữu</t>
   </si>
 </sst>
 </file>
@@ -11457,7 +11562,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11984,10 +12099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B3878"/>
+  <dimension ref="A1:B3913"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3866" workbookViewId="0">
-      <selection activeCell="G3882" sqref="G3882"/>
+    <sheetView tabSelected="1" topLeftCell="A3851" workbookViewId="0">
+      <selection activeCell="F3858" sqref="F3858"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42995,61 +43110,341 @@
         <v>3796</v>
       </c>
     </row>
+    <row r="3879" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3879" t="s">
+        <v>3797</v>
+      </c>
+      <c r="B3879" t="s">
+        <v>3797</v>
+      </c>
+    </row>
+    <row r="3880" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3880" t="s">
+        <v>3798</v>
+      </c>
+      <c r="B3880" t="s">
+        <v>3798</v>
+      </c>
+    </row>
+    <row r="3881" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3881" t="s">
+        <v>3799</v>
+      </c>
+      <c r="B3881" t="s">
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="3882" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3882" t="s">
+        <v>3800</v>
+      </c>
+      <c r="B3882" t="s">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="3883" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3883" t="s">
+        <v>3801</v>
+      </c>
+      <c r="B3883" t="s">
+        <v>3801</v>
+      </c>
+    </row>
+    <row r="3884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3884" t="s">
+        <v>3802</v>
+      </c>
+      <c r="B3884" t="s">
+        <v>3802</v>
+      </c>
+    </row>
+    <row r="3885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3885" t="s">
+        <v>3803</v>
+      </c>
+      <c r="B3885" t="s">
+        <v>3803</v>
+      </c>
+    </row>
+    <row r="3886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3886" t="s">
+        <v>3804</v>
+      </c>
+      <c r="B3886" t="s">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="3887" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3887" t="s">
+        <v>3805</v>
+      </c>
+      <c r="B3887" t="s">
+        <v>3805</v>
+      </c>
+    </row>
+    <row r="3888" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3888" t="s">
+        <v>3806</v>
+      </c>
+      <c r="B3888" t="s">
+        <v>3806</v>
+      </c>
+    </row>
+    <row r="3889" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3889" t="s">
+        <v>3807</v>
+      </c>
+      <c r="B3889" t="s">
+        <v>3807</v>
+      </c>
+    </row>
+    <row r="3890" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3890" t="s">
+        <v>3808</v>
+      </c>
+      <c r="B3890" t="s">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="3891" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3891" t="s">
+        <v>3809</v>
+      </c>
+      <c r="B3891" t="s">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="3892" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3892" t="s">
+        <v>3810</v>
+      </c>
+      <c r="B3892" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="3893" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3893" t="s">
+        <v>3811</v>
+      </c>
+      <c r="B3893" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="3894" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3894" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B3894" t="s">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="3895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3895" t="s">
+        <v>3813</v>
+      </c>
+      <c r="B3895" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="3896" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3896" t="s">
+        <v>3814</v>
+      </c>
+      <c r="B3896" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="3897" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3897" t="s">
+        <v>3815</v>
+      </c>
+      <c r="B3897" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="3898" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3898" t="s">
+        <v>3816</v>
+      </c>
+      <c r="B3898" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="3899" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3899" t="s">
+        <v>3817</v>
+      </c>
+      <c r="B3899" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="3900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3900" t="s">
+        <v>3818</v>
+      </c>
+      <c r="B3900" t="s">
+        <v>3818</v>
+      </c>
+    </row>
+    <row r="3901" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3901" t="s">
+        <v>3819</v>
+      </c>
+      <c r="B3901" t="s">
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="3902" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3902" t="s">
+        <v>3820</v>
+      </c>
+      <c r="B3902" t="s">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="3903" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3903" t="s">
+        <v>3821</v>
+      </c>
+      <c r="B3903" t="s">
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="3904" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3904" t="s">
+        <v>3822</v>
+      </c>
+      <c r="B3904" t="s">
+        <v>3822</v>
+      </c>
+    </row>
+    <row r="3905" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3905" t="s">
+        <v>3823</v>
+      </c>
+      <c r="B3905" t="s">
+        <v>3823</v>
+      </c>
+    </row>
+    <row r="3906" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3906" t="s">
+        <v>3824</v>
+      </c>
+      <c r="B3906" t="s">
+        <v>3824</v>
+      </c>
+    </row>
+    <row r="3907" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3907" t="s">
+        <v>3825</v>
+      </c>
+      <c r="B3907" t="s">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="3908" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3908" t="s">
+        <v>3826</v>
+      </c>
+      <c r="B3908" t="s">
+        <v>3826</v>
+      </c>
+    </row>
+    <row r="3909" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3909" t="s">
+        <v>3827</v>
+      </c>
+      <c r="B3909" t="s">
+        <v>3827</v>
+      </c>
+    </row>
+    <row r="3910" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3910" t="s">
+        <v>3828</v>
+      </c>
+      <c r="B3910" t="s">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="3911" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3911" t="s">
+        <v>3829</v>
+      </c>
+      <c r="B3911" t="s">
+        <v>3829</v>
+      </c>
+    </row>
+    <row r="3912" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3912" t="s">
+        <v>3830</v>
+      </c>
+      <c r="B3912" t="s">
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="3913" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3913" t="s">
+        <v>3831</v>
+      </c>
+      <c r="B3913" t="s">
+        <v>3831</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="24" priority="71"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="72"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="22" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="20" priority="45"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="18" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="41"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3851 A3879:A1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="80"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="82"/>
+  <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3851 A3914:A1048576">
+    <cfRule type="duplicateValues" dxfId="18" priority="81"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="83"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="15" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="14" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209:B1631 B1:B23 B25:B84 B143">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1805:B1809 B3442:B3813 B3851 B3879:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="22"/>
+  <conditionalFormatting sqref="B1805:B1809 B3442:B3813 B3851 B3914:B1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1810:B3339">
-    <cfRule type="duplicateValues" dxfId="3" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3814:B3850">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3852:A3878">
+  <conditionalFormatting sqref="A3852:A3913">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Thêm luận cách cục 12 cung vào
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACEF48F-EC9F-482C-A889-B39CC68E0D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC6227E-1562-47C9-99CB-E284F04BBA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8488" uniqueCount="4244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8646" uniqueCount="4323">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -12757,6 +12757,243 @@
   </si>
   <si>
     <t>L. Đà La tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Sát Phá Tham hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Phủ Vũ Tướng hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cự Nhật hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Kình Đà hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Xương Khúc hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hoả Linh hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Không Kiếp hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Quang Quý hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tả Hữu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Song Hao hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tang Hổ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Khốc Hư hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hình Riêu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thai Toạ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Ấn Phù hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Song Hao Quyền Lộc Kiếp Hoả hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Phủ Vũ Tướng Xương Khúc Khôi Việt Tả Hữu Khoa Quyền Lộc Long hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Phủ Vũ Tướng Tả Hữu Khoa Quyền Lộc Long Phượng hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Khúc Phá Dương Đà hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương gặp Xương Khúc Tả Hữu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương Khoa Tả Hữu Quang Quý Quan Phúc hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Sát Quyền hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Lộc Mã hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Kiếp Hư Hao Quyền hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tuế Hổ Phù Xương Khúc hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Xương Khúc Tấu Long Phượng hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Riêu Tấu Cơ Vũ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Binh Hình Tướng Ấn hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hổ Tấu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hình Riêu Y hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Mã Hỏa Linh hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thai Tọa Hồng Đào hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tả Hữu Không Kiếp hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tả Hữu Binh Tướng hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Quyền hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Tả Cái Hữu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Quan Phúc Quang Tấu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Xương Khúc hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Tử Phủ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hổ Kình Sát hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hổ Tang Kiếp hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hổ Tang Không Kiếp hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Âm Dương Lương hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cơ Lương Gia Hội hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Nhật Chiếu Lôi Môn hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tả Hữu Xương Khúc hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tham Linh Triều Viên hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cự Hỏa Linh hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Hồng Đào Kỵ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cự Đồng Hình hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Lương Phá hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Khôi Việt hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tham Vũ Hỏa hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cự Kỵ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Kình Đà Hỏa hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Kình Đà Không Kiếp hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Hỷ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Kiếp Sát hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Kỵ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Tả Phù Hữu Bật hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Tả Phù Hữu Bật Khoa Quyền Lộc hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đào Hồng Tả Phù Hữu Bật Khoa Quyền Lộc Long Trì Phượng Các hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Lưu Hà Kiếp Sát hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Phục Không Kiếp hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Xương Khúc Khôi Việt hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Khoa Quyền hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Lộc Quyền hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tướng Binh Đào Hồng hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Lương Khốc Tuế hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tướng Binh hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cự Tang hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cự Hỏa hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Phá Hình Kỵ hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tang Trực Tuế hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tuế Xương Khúc hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Vi Tả Hữu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Vi Tang Tả Hữu hội chiếu tại Điền Trạch</t>
   </si>
 </sst>
 </file>
@@ -12798,117 +13035,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13405,10 +13532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4245"/>
+  <dimension ref="A1:B4325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4212" workbookViewId="0">
-      <selection activeCell="B4191" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4218" workbookViewId="0">
+      <selection activeCell="B4247" sqref="B4247:B4325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47365,32 +47492,664 @@
         <v>4243</v>
       </c>
     </row>
+    <row r="4247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4247" t="s">
+        <v>4244</v>
+      </c>
+      <c r="B4247" t="s">
+        <v>4244</v>
+      </c>
+    </row>
+    <row r="4248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4248" t="s">
+        <v>4245</v>
+      </c>
+      <c r="B4248" t="s">
+        <v>4245</v>
+      </c>
+    </row>
+    <row r="4249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4249" t="s">
+        <v>4246</v>
+      </c>
+      <c r="B4249" t="s">
+        <v>4246</v>
+      </c>
+    </row>
+    <row r="4250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4250" t="s">
+        <v>4247</v>
+      </c>
+      <c r="B4250" t="s">
+        <v>4247</v>
+      </c>
+    </row>
+    <row r="4251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4251" t="s">
+        <v>4248</v>
+      </c>
+      <c r="B4251" t="s">
+        <v>4248</v>
+      </c>
+    </row>
+    <row r="4252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4252" t="s">
+        <v>4249</v>
+      </c>
+      <c r="B4252" t="s">
+        <v>4249</v>
+      </c>
+    </row>
+    <row r="4253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4253" t="s">
+        <v>4250</v>
+      </c>
+      <c r="B4253" t="s">
+        <v>4250</v>
+      </c>
+    </row>
+    <row r="4254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4254" t="s">
+        <v>4251</v>
+      </c>
+      <c r="B4254" t="s">
+        <v>4251</v>
+      </c>
+    </row>
+    <row r="4255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4255" t="s">
+        <v>4252</v>
+      </c>
+      <c r="B4255" t="s">
+        <v>4252</v>
+      </c>
+    </row>
+    <row r="4256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4256" t="s">
+        <v>4253</v>
+      </c>
+      <c r="B4256" t="s">
+        <v>4253</v>
+      </c>
+    </row>
+    <row r="4257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4257" t="s">
+        <v>4254</v>
+      </c>
+      <c r="B4257" t="s">
+        <v>4254</v>
+      </c>
+    </row>
+    <row r="4258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4258" t="s">
+        <v>4255</v>
+      </c>
+      <c r="B4258" t="s">
+        <v>4255</v>
+      </c>
+    </row>
+    <row r="4259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4259" t="s">
+        <v>4256</v>
+      </c>
+      <c r="B4259" t="s">
+        <v>4256</v>
+      </c>
+    </row>
+    <row r="4260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4260" t="s">
+        <v>4257</v>
+      </c>
+      <c r="B4260" t="s">
+        <v>4257</v>
+      </c>
+    </row>
+    <row r="4261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4261" t="s">
+        <v>4258</v>
+      </c>
+      <c r="B4261" t="s">
+        <v>4258</v>
+      </c>
+    </row>
+    <row r="4262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4262" t="s">
+        <v>4259</v>
+      </c>
+      <c r="B4262" t="s">
+        <v>4259</v>
+      </c>
+    </row>
+    <row r="4263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4263" t="s">
+        <v>4260</v>
+      </c>
+      <c r="B4263" t="s">
+        <v>4260</v>
+      </c>
+    </row>
+    <row r="4264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4264" t="s">
+        <v>4261</v>
+      </c>
+      <c r="B4264" t="s">
+        <v>4261</v>
+      </c>
+    </row>
+    <row r="4265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4265" t="s">
+        <v>4262</v>
+      </c>
+      <c r="B4265" t="s">
+        <v>4262</v>
+      </c>
+    </row>
+    <row r="4266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4266" t="s">
+        <v>4263</v>
+      </c>
+      <c r="B4266" t="s">
+        <v>4263</v>
+      </c>
+    </row>
+    <row r="4267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4267" t="s">
+        <v>4264</v>
+      </c>
+      <c r="B4267" t="s">
+        <v>4264</v>
+      </c>
+    </row>
+    <row r="4268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4268" t="s">
+        <v>4265</v>
+      </c>
+      <c r="B4268" t="s">
+        <v>4265</v>
+      </c>
+    </row>
+    <row r="4269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4269" t="s">
+        <v>4266</v>
+      </c>
+      <c r="B4269" t="s">
+        <v>4266</v>
+      </c>
+    </row>
+    <row r="4270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4270" t="s">
+        <v>4267</v>
+      </c>
+      <c r="B4270" t="s">
+        <v>4267</v>
+      </c>
+    </row>
+    <row r="4271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4271" t="s">
+        <v>4268</v>
+      </c>
+      <c r="B4271" t="s">
+        <v>4268</v>
+      </c>
+    </row>
+    <row r="4272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4272" t="s">
+        <v>4269</v>
+      </c>
+      <c r="B4272" t="s">
+        <v>4269</v>
+      </c>
+    </row>
+    <row r="4273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4273" t="s">
+        <v>4270</v>
+      </c>
+      <c r="B4273" t="s">
+        <v>4270</v>
+      </c>
+    </row>
+    <row r="4274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4274" t="s">
+        <v>4271</v>
+      </c>
+      <c r="B4274" t="s">
+        <v>4271</v>
+      </c>
+    </row>
+    <row r="4275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4275" t="s">
+        <v>4272</v>
+      </c>
+      <c r="B4275" t="s">
+        <v>4272</v>
+      </c>
+    </row>
+    <row r="4276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4276" t="s">
+        <v>4273</v>
+      </c>
+      <c r="B4276" t="s">
+        <v>4273</v>
+      </c>
+    </row>
+    <row r="4277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4277" t="s">
+        <v>4274</v>
+      </c>
+      <c r="B4277" t="s">
+        <v>4274</v>
+      </c>
+    </row>
+    <row r="4278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4278" t="s">
+        <v>4275</v>
+      </c>
+      <c r="B4278" t="s">
+        <v>4275</v>
+      </c>
+    </row>
+    <row r="4279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4279" t="s">
+        <v>4276</v>
+      </c>
+      <c r="B4279" t="s">
+        <v>4276</v>
+      </c>
+    </row>
+    <row r="4280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4280" t="s">
+        <v>4277</v>
+      </c>
+      <c r="B4280" t="s">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="4281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4281" t="s">
+        <v>4278</v>
+      </c>
+      <c r="B4281" t="s">
+        <v>4278</v>
+      </c>
+    </row>
+    <row r="4282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4282" t="s">
+        <v>4279</v>
+      </c>
+      <c r="B4282" t="s">
+        <v>4279</v>
+      </c>
+    </row>
+    <row r="4283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4283" t="s">
+        <v>4280</v>
+      </c>
+      <c r="B4283" t="s">
+        <v>4280</v>
+      </c>
+    </row>
+    <row r="4284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4284" t="s">
+        <v>4281</v>
+      </c>
+      <c r="B4284" t="s">
+        <v>4281</v>
+      </c>
+    </row>
+    <row r="4285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4285" t="s">
+        <v>4282</v>
+      </c>
+      <c r="B4285" t="s">
+        <v>4282</v>
+      </c>
+    </row>
+    <row r="4286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4286" t="s">
+        <v>4283</v>
+      </c>
+      <c r="B4286" t="s">
+        <v>4283</v>
+      </c>
+    </row>
+    <row r="4287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4287" t="s">
+        <v>4284</v>
+      </c>
+      <c r="B4287" t="s">
+        <v>4284</v>
+      </c>
+    </row>
+    <row r="4288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4288" t="s">
+        <v>4285</v>
+      </c>
+      <c r="B4288" t="s">
+        <v>4285</v>
+      </c>
+    </row>
+    <row r="4289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4289" t="s">
+        <v>4286</v>
+      </c>
+      <c r="B4289" t="s">
+        <v>4286</v>
+      </c>
+    </row>
+    <row r="4290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4290" t="s">
+        <v>4287</v>
+      </c>
+      <c r="B4290" t="s">
+        <v>4287</v>
+      </c>
+    </row>
+    <row r="4291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4291" t="s">
+        <v>4288</v>
+      </c>
+      <c r="B4291" t="s">
+        <v>4288</v>
+      </c>
+    </row>
+    <row r="4292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4292" t="s">
+        <v>4289</v>
+      </c>
+      <c r="B4292" t="s">
+        <v>4289</v>
+      </c>
+    </row>
+    <row r="4293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4293" t="s">
+        <v>4290</v>
+      </c>
+      <c r="B4293" t="s">
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="4294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4294" t="s">
+        <v>4291</v>
+      </c>
+      <c r="B4294" t="s">
+        <v>4291</v>
+      </c>
+    </row>
+    <row r="4295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4295" t="s">
+        <v>4292</v>
+      </c>
+      <c r="B4295" t="s">
+        <v>4292</v>
+      </c>
+    </row>
+    <row r="4296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4296" t="s">
+        <v>4293</v>
+      </c>
+      <c r="B4296" t="s">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="4297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4297" t="s">
+        <v>4294</v>
+      </c>
+      <c r="B4297" t="s">
+        <v>4294</v>
+      </c>
+    </row>
+    <row r="4298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4298" t="s">
+        <v>4295</v>
+      </c>
+      <c r="B4298" t="s">
+        <v>4295</v>
+      </c>
+    </row>
+    <row r="4299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4299" t="s">
+        <v>4296</v>
+      </c>
+      <c r="B4299" t="s">
+        <v>4296</v>
+      </c>
+    </row>
+    <row r="4300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4300" t="s">
+        <v>4297</v>
+      </c>
+      <c r="B4300" t="s">
+        <v>4297</v>
+      </c>
+    </row>
+    <row r="4301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4301" t="s">
+        <v>4298</v>
+      </c>
+      <c r="B4301" t="s">
+        <v>4298</v>
+      </c>
+    </row>
+    <row r="4302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4302" t="s">
+        <v>4299</v>
+      </c>
+      <c r="B4302" t="s">
+        <v>4299</v>
+      </c>
+    </row>
+    <row r="4303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4303" t="s">
+        <v>4300</v>
+      </c>
+      <c r="B4303" t="s">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="4304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4304" t="s">
+        <v>4301</v>
+      </c>
+      <c r="B4304" t="s">
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="4305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4305" t="s">
+        <v>4302</v>
+      </c>
+      <c r="B4305" t="s">
+        <v>4302</v>
+      </c>
+    </row>
+    <row r="4306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4306" t="s">
+        <v>4303</v>
+      </c>
+      <c r="B4306" t="s">
+        <v>4303</v>
+      </c>
+    </row>
+    <row r="4307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4307" t="s">
+        <v>4304</v>
+      </c>
+      <c r="B4307" t="s">
+        <v>4304</v>
+      </c>
+    </row>
+    <row r="4308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4308" t="s">
+        <v>4305</v>
+      </c>
+      <c r="B4308" t="s">
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="4309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4309" t="s">
+        <v>4306</v>
+      </c>
+      <c r="B4309" t="s">
+        <v>4306</v>
+      </c>
+    </row>
+    <row r="4310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4310" t="s">
+        <v>4307</v>
+      </c>
+      <c r="B4310" t="s">
+        <v>4307</v>
+      </c>
+    </row>
+    <row r="4311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4311" t="s">
+        <v>4308</v>
+      </c>
+      <c r="B4311" t="s">
+        <v>4308</v>
+      </c>
+    </row>
+    <row r="4312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4312" t="s">
+        <v>4309</v>
+      </c>
+      <c r="B4312" t="s">
+        <v>4309</v>
+      </c>
+    </row>
+    <row r="4313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4313" t="s">
+        <v>4310</v>
+      </c>
+      <c r="B4313" t="s">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="4314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4314" t="s">
+        <v>4311</v>
+      </c>
+      <c r="B4314" t="s">
+        <v>4311</v>
+      </c>
+    </row>
+    <row r="4315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4315" t="s">
+        <v>4312</v>
+      </c>
+      <c r="B4315" t="s">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="4316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4316" t="s">
+        <v>4313</v>
+      </c>
+      <c r="B4316" t="s">
+        <v>4313</v>
+      </c>
+    </row>
+    <row r="4317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4317" t="s">
+        <v>4314</v>
+      </c>
+      <c r="B4317" t="s">
+        <v>4314</v>
+      </c>
+    </row>
+    <row r="4318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4318" t="s">
+        <v>4315</v>
+      </c>
+      <c r="B4318" t="s">
+        <v>4315</v>
+      </c>
+    </row>
+    <row r="4319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4319" t="s">
+        <v>4316</v>
+      </c>
+      <c r="B4319" t="s">
+        <v>4316</v>
+      </c>
+    </row>
+    <row r="4320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4320" t="s">
+        <v>4317</v>
+      </c>
+      <c r="B4320" t="s">
+        <v>4317</v>
+      </c>
+    </row>
+    <row r="4321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4321" t="s">
+        <v>4318</v>
+      </c>
+      <c r="B4321" t="s">
+        <v>4318</v>
+      </c>
+    </row>
+    <row r="4322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4322" t="s">
+        <v>4319</v>
+      </c>
+      <c r="B4322" t="s">
+        <v>4319</v>
+      </c>
+    </row>
+    <row r="4323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4323" t="s">
+        <v>4320</v>
+      </c>
+      <c r="B4323" t="s">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="4324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4324" t="s">
+        <v>4321</v>
+      </c>
+      <c r="B4324" t="s">
+        <v>4321</v>
+      </c>
+    </row>
+    <row r="4325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4325" t="s">
+        <v>4322</v>
+      </c>
+      <c r="B4325" t="s">
+        <v>4322</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="32" priority="94"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="95"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="94"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="95"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="30" priority="64"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="28" priority="68"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="26" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1809 A3442:A3851 A3914:A4212 A6758:A1048576">
-    <cfRule type="duplicateValues" dxfId="25" priority="103"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="105"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="103"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="105"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1810:A3339">
-    <cfRule type="duplicateValues" dxfId="23" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3852:A3913">
-    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
     <cfRule type="duplicateValues" dxfId="10" priority="8"/>

</xml_diff>

<commit_message>
Luận thêm phần đối của cung vô chính diệu
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC6227E-1562-47C9-99CB-E284F04BBA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59E1D01-A107-4209-A1AD-682407CE1837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8646" uniqueCount="4323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8856" uniqueCount="4428">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -12994,6 +12994,321 @@
   </si>
   <si>
     <t>Tử Vi Tang Tả Hữu hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Âm tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tham Lang tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Cự Môn tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Lương tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thất Sát tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Cơ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thái Dương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Vũ Khúc tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Đồng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Liêm Trinh tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Phủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thái Âm tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thái Dương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Vũ Khúc tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thiên Đồng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Liêm Trinh tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thiên Phủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thái Âm tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Vũ Khúc tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Thiên Đồng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Liêm Trinh tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Thiên Phủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Thái Âm tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Dương đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Thiên Đồng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Liêm Trinh tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Thiên Phủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Thái Âm tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Vũ Khúc đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Liêm Trinh tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Thiên Phủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Thái Âm tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Phủ tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thái Âm tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung Thái Âm tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Phủ đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Âm đồng cung Tham Lang tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Âm đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Âm đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Âm đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Âm đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Âm đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tham Lang đồng cung Cự Môn tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tham Lang đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tham Lang đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tham Lang đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Tham Lang đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Cự Môn đồng cung Thiên Tướng tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Cự Môn đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Cự Môn đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Cự Môn đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Tướng đồng cung Thiên Lương tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Tướng đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Tướng đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Lương đồng cung Thất Sát tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Lương đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Thất Sát đồng cung Phá Quân tại cung đối Tử Tức</t>
   </si>
 </sst>
 </file>
@@ -13532,10 +13847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4325"/>
+  <dimension ref="A1:B4432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4218" workbookViewId="0">
-      <selection activeCell="B4247" sqref="B4247:B4325"/>
+    <sheetView tabSelected="1" topLeftCell="A4317" workbookViewId="0">
+      <selection activeCell="B4342" sqref="B4342:B4432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48122,6 +48437,846 @@
       </c>
       <c r="B4325" t="s">
         <v>4322</v>
+      </c>
+    </row>
+    <row r="4327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4327" t="s">
+        <v>4323</v>
+      </c>
+      <c r="B4327" t="s">
+        <v>4323</v>
+      </c>
+    </row>
+    <row r="4328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4328" t="s">
+        <v>4324</v>
+      </c>
+      <c r="B4328" t="s">
+        <v>4324</v>
+      </c>
+    </row>
+    <row r="4329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4329" t="s">
+        <v>4325</v>
+      </c>
+      <c r="B4329" t="s">
+        <v>4325</v>
+      </c>
+    </row>
+    <row r="4330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4330" t="s">
+        <v>4326</v>
+      </c>
+      <c r="B4330" t="s">
+        <v>4326</v>
+      </c>
+    </row>
+    <row r="4331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4331" t="s">
+        <v>4327</v>
+      </c>
+      <c r="B4331" t="s">
+        <v>4327</v>
+      </c>
+    </row>
+    <row r="4332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4332" t="s">
+        <v>4328</v>
+      </c>
+      <c r="B4332" t="s">
+        <v>4328</v>
+      </c>
+    </row>
+    <row r="4333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4333" t="s">
+        <v>4329</v>
+      </c>
+      <c r="B4333" t="s">
+        <v>4329</v>
+      </c>
+    </row>
+    <row r="4334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4334" t="s">
+        <v>4330</v>
+      </c>
+      <c r="B4334" t="s">
+        <v>4330</v>
+      </c>
+    </row>
+    <row r="4335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4335" t="s">
+        <v>4331</v>
+      </c>
+      <c r="B4335" t="s">
+        <v>4331</v>
+      </c>
+    </row>
+    <row r="4336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4336" t="s">
+        <v>4332</v>
+      </c>
+      <c r="B4336" t="s">
+        <v>4332</v>
+      </c>
+    </row>
+    <row r="4337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4337" t="s">
+        <v>4333</v>
+      </c>
+      <c r="B4337" t="s">
+        <v>4333</v>
+      </c>
+    </row>
+    <row r="4338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4338" t="s">
+        <v>4334</v>
+      </c>
+      <c r="B4338" t="s">
+        <v>4334</v>
+      </c>
+    </row>
+    <row r="4339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4339" t="s">
+        <v>4335</v>
+      </c>
+      <c r="B4339" t="s">
+        <v>4335</v>
+      </c>
+    </row>
+    <row r="4340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4340" t="s">
+        <v>4336</v>
+      </c>
+      <c r="B4340" t="s">
+        <v>4336</v>
+      </c>
+    </row>
+    <row r="4342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4342" t="s">
+        <v>4337</v>
+      </c>
+      <c r="B4342" t="s">
+        <v>4337</v>
+      </c>
+    </row>
+    <row r="4343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4343" t="s">
+        <v>4338</v>
+      </c>
+      <c r="B4343" t="s">
+        <v>4338</v>
+      </c>
+    </row>
+    <row r="4344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4344" t="s">
+        <v>4339</v>
+      </c>
+      <c r="B4344" t="s">
+        <v>4339</v>
+      </c>
+    </row>
+    <row r="4345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4345" t="s">
+        <v>4340</v>
+      </c>
+      <c r="B4345" t="s">
+        <v>4340</v>
+      </c>
+    </row>
+    <row r="4346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4346" t="s">
+        <v>4341</v>
+      </c>
+      <c r="B4346" t="s">
+        <v>4341</v>
+      </c>
+    </row>
+    <row r="4347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4347" t="s">
+        <v>4342</v>
+      </c>
+      <c r="B4347" t="s">
+        <v>4342</v>
+      </c>
+    </row>
+    <row r="4348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4348" t="s">
+        <v>4343</v>
+      </c>
+      <c r="B4348" t="s">
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="4349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4349" t="s">
+        <v>4344</v>
+      </c>
+      <c r="B4349" t="s">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="4350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4350" t="s">
+        <v>4345</v>
+      </c>
+      <c r="B4350" t="s">
+        <v>4345</v>
+      </c>
+    </row>
+    <row r="4351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4351" t="s">
+        <v>4346</v>
+      </c>
+      <c r="B4351" t="s">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="4352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4352" t="s">
+        <v>4347</v>
+      </c>
+      <c r="B4352" t="s">
+        <v>4347</v>
+      </c>
+    </row>
+    <row r="4353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4353" t="s">
+        <v>4348</v>
+      </c>
+      <c r="B4353" t="s">
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="4354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4354" t="s">
+        <v>4349</v>
+      </c>
+      <c r="B4354" t="s">
+        <v>4349</v>
+      </c>
+    </row>
+    <row r="4355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4355" t="s">
+        <v>4350</v>
+      </c>
+      <c r="B4355" t="s">
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="4356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4356" t="s">
+        <v>4351</v>
+      </c>
+      <c r="B4356" t="s">
+        <v>4351</v>
+      </c>
+    </row>
+    <row r="4357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4357" t="s">
+        <v>4352</v>
+      </c>
+      <c r="B4357" t="s">
+        <v>4352</v>
+      </c>
+    </row>
+    <row r="4358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4358" t="s">
+        <v>4353</v>
+      </c>
+      <c r="B4358" t="s">
+        <v>4353</v>
+      </c>
+    </row>
+    <row r="4359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4359" t="s">
+        <v>4354</v>
+      </c>
+      <c r="B4359" t="s">
+        <v>4354</v>
+      </c>
+    </row>
+    <row r="4360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4360" t="s">
+        <v>4355</v>
+      </c>
+      <c r="B4360" t="s">
+        <v>4355</v>
+      </c>
+    </row>
+    <row r="4361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4361" t="s">
+        <v>4356</v>
+      </c>
+      <c r="B4361" t="s">
+        <v>4356</v>
+      </c>
+    </row>
+    <row r="4362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4362" t="s">
+        <v>4357</v>
+      </c>
+      <c r="B4362" t="s">
+        <v>4357</v>
+      </c>
+    </row>
+    <row r="4363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4363" t="s">
+        <v>4358</v>
+      </c>
+      <c r="B4363" t="s">
+        <v>4358</v>
+      </c>
+    </row>
+    <row r="4364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4364" t="s">
+        <v>4359</v>
+      </c>
+      <c r="B4364" t="s">
+        <v>4359</v>
+      </c>
+    </row>
+    <row r="4365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4365" t="s">
+        <v>4360</v>
+      </c>
+      <c r="B4365" t="s">
+        <v>4360</v>
+      </c>
+    </row>
+    <row r="4366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4366" t="s">
+        <v>4361</v>
+      </c>
+      <c r="B4366" t="s">
+        <v>4361</v>
+      </c>
+    </row>
+    <row r="4367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4367" t="s">
+        <v>4362</v>
+      </c>
+      <c r="B4367" t="s">
+        <v>4362</v>
+      </c>
+    </row>
+    <row r="4368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4368" t="s">
+        <v>4363</v>
+      </c>
+      <c r="B4368" t="s">
+        <v>4363</v>
+      </c>
+    </row>
+    <row r="4369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4369" t="s">
+        <v>4364</v>
+      </c>
+      <c r="B4369" t="s">
+        <v>4364</v>
+      </c>
+    </row>
+    <row r="4370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4370" t="s">
+        <v>4365</v>
+      </c>
+      <c r="B4370" t="s">
+        <v>4365</v>
+      </c>
+    </row>
+    <row r="4371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4371" t="s">
+        <v>4366</v>
+      </c>
+      <c r="B4371" t="s">
+        <v>4366</v>
+      </c>
+    </row>
+    <row r="4372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4372" t="s">
+        <v>4367</v>
+      </c>
+      <c r="B4372" t="s">
+        <v>4367</v>
+      </c>
+    </row>
+    <row r="4373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4373" t="s">
+        <v>4368</v>
+      </c>
+      <c r="B4373" t="s">
+        <v>4368</v>
+      </c>
+    </row>
+    <row r="4374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4374" t="s">
+        <v>4369</v>
+      </c>
+      <c r="B4374" t="s">
+        <v>4369</v>
+      </c>
+    </row>
+    <row r="4375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4375" t="s">
+        <v>4370</v>
+      </c>
+      <c r="B4375" t="s">
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="4376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4376" t="s">
+        <v>4371</v>
+      </c>
+      <c r="B4376" t="s">
+        <v>4371</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4377" t="s">
+        <v>4372</v>
+      </c>
+      <c r="B4377" t="s">
+        <v>4372</v>
+      </c>
+    </row>
+    <row r="4378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4378" t="s">
+        <v>4373</v>
+      </c>
+      <c r="B4378" t="s">
+        <v>4373</v>
+      </c>
+    </row>
+    <row r="4379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4379" t="s">
+        <v>4374</v>
+      </c>
+      <c r="B4379" t="s">
+        <v>4374</v>
+      </c>
+    </row>
+    <row r="4380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4380" t="s">
+        <v>4375</v>
+      </c>
+      <c r="B4380" t="s">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="4381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4381" t="s">
+        <v>4376</v>
+      </c>
+      <c r="B4381" t="s">
+        <v>4376</v>
+      </c>
+    </row>
+    <row r="4382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4382" t="s">
+        <v>4377</v>
+      </c>
+      <c r="B4382" t="s">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="4383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4383" t="s">
+        <v>4378</v>
+      </c>
+      <c r="B4383" t="s">
+        <v>4378</v>
+      </c>
+    </row>
+    <row r="4384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4384" t="s">
+        <v>4379</v>
+      </c>
+      <c r="B4384" t="s">
+        <v>4379</v>
+      </c>
+    </row>
+    <row r="4385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4385" t="s">
+        <v>4380</v>
+      </c>
+      <c r="B4385" t="s">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="4386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4386" t="s">
+        <v>4381</v>
+      </c>
+      <c r="B4386" t="s">
+        <v>4381</v>
+      </c>
+    </row>
+    <row r="4387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4387" t="s">
+        <v>4382</v>
+      </c>
+      <c r="B4387" t="s">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="4388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4388" t="s">
+        <v>4383</v>
+      </c>
+      <c r="B4388" t="s">
+        <v>4383</v>
+      </c>
+    </row>
+    <row r="4389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4389" t="s">
+        <v>4384</v>
+      </c>
+      <c r="B4389" t="s">
+        <v>4384</v>
+      </c>
+    </row>
+    <row r="4390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4390" t="s">
+        <v>4385</v>
+      </c>
+      <c r="B4390" t="s">
+        <v>4385</v>
+      </c>
+    </row>
+    <row r="4391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4391" t="s">
+        <v>4386</v>
+      </c>
+      <c r="B4391" t="s">
+        <v>4386</v>
+      </c>
+    </row>
+    <row r="4392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4392" t="s">
+        <v>4387</v>
+      </c>
+      <c r="B4392" t="s">
+        <v>4387</v>
+      </c>
+    </row>
+    <row r="4393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4393" t="s">
+        <v>4388</v>
+      </c>
+      <c r="B4393" t="s">
+        <v>4388</v>
+      </c>
+    </row>
+    <row r="4394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4394" t="s">
+        <v>4389</v>
+      </c>
+      <c r="B4394" t="s">
+        <v>4389</v>
+      </c>
+    </row>
+    <row r="4395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4395" t="s">
+        <v>4390</v>
+      </c>
+      <c r="B4395" t="s">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="4396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4396" t="s">
+        <v>4391</v>
+      </c>
+      <c r="B4396" t="s">
+        <v>4391</v>
+      </c>
+    </row>
+    <row r="4397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4397" t="s">
+        <v>4392</v>
+      </c>
+      <c r="B4397" t="s">
+        <v>4392</v>
+      </c>
+    </row>
+    <row r="4398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4398" t="s">
+        <v>4393</v>
+      </c>
+      <c r="B4398" t="s">
+        <v>4393</v>
+      </c>
+    </row>
+    <row r="4399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4399" t="s">
+        <v>4394</v>
+      </c>
+      <c r="B4399" t="s">
+        <v>4394</v>
+      </c>
+    </row>
+    <row r="4400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4400" t="s">
+        <v>4395</v>
+      </c>
+      <c r="B4400" t="s">
+        <v>4395</v>
+      </c>
+    </row>
+    <row r="4401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4401" t="s">
+        <v>4396</v>
+      </c>
+      <c r="B4401" t="s">
+        <v>4396</v>
+      </c>
+    </row>
+    <row r="4402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4402" t="s">
+        <v>4397</v>
+      </c>
+      <c r="B4402" t="s">
+        <v>4397</v>
+      </c>
+    </row>
+    <row r="4403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4403" t="s">
+        <v>4398</v>
+      </c>
+      <c r="B4403" t="s">
+        <v>4398</v>
+      </c>
+    </row>
+    <row r="4404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4404" t="s">
+        <v>4399</v>
+      </c>
+      <c r="B4404" t="s">
+        <v>4399</v>
+      </c>
+    </row>
+    <row r="4405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4405" t="s">
+        <v>4400</v>
+      </c>
+      <c r="B4405" t="s">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="4406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4406" t="s">
+        <v>4401</v>
+      </c>
+      <c r="B4406" t="s">
+        <v>4401</v>
+      </c>
+    </row>
+    <row r="4407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4407" t="s">
+        <v>4402</v>
+      </c>
+      <c r="B4407" t="s">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="4408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4408" t="s">
+        <v>4403</v>
+      </c>
+      <c r="B4408" t="s">
+        <v>4403</v>
+      </c>
+    </row>
+    <row r="4409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4409" t="s">
+        <v>4404</v>
+      </c>
+      <c r="B4409" t="s">
+        <v>4404</v>
+      </c>
+    </row>
+    <row r="4410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4410" t="s">
+        <v>4405</v>
+      </c>
+      <c r="B4410" t="s">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="4411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4411" t="s">
+        <v>4406</v>
+      </c>
+      <c r="B4411" t="s">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="4412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4412" t="s">
+        <v>4407</v>
+      </c>
+      <c r="B4412" t="s">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="4413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4413" t="s">
+        <v>4408</v>
+      </c>
+      <c r="B4413" t="s">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="4414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4414" t="s">
+        <v>4409</v>
+      </c>
+      <c r="B4414" t="s">
+        <v>4409</v>
+      </c>
+    </row>
+    <row r="4415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4415" t="s">
+        <v>4410</v>
+      </c>
+      <c r="B4415" t="s">
+        <v>4410</v>
+      </c>
+    </row>
+    <row r="4416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4416" t="s">
+        <v>4411</v>
+      </c>
+      <c r="B4416" t="s">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="4417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4417" t="s">
+        <v>4412</v>
+      </c>
+      <c r="B4417" t="s">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="4418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4418" t="s">
+        <v>4413</v>
+      </c>
+      <c r="B4418" t="s">
+        <v>4413</v>
+      </c>
+    </row>
+    <row r="4419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4419" t="s">
+        <v>4414</v>
+      </c>
+      <c r="B4419" t="s">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="4420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4420" t="s">
+        <v>4415</v>
+      </c>
+      <c r="B4420" t="s">
+        <v>4415</v>
+      </c>
+    </row>
+    <row r="4421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4421" t="s">
+        <v>4416</v>
+      </c>
+      <c r="B4421" t="s">
+        <v>4416</v>
+      </c>
+    </row>
+    <row r="4422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4422" t="s">
+        <v>4417</v>
+      </c>
+      <c r="B4422" t="s">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="4423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4423" t="s">
+        <v>4418</v>
+      </c>
+      <c r="B4423" t="s">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="4424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4424" t="s">
+        <v>4419</v>
+      </c>
+      <c r="B4424" t="s">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="4425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4425" t="s">
+        <v>4420</v>
+      </c>
+      <c r="B4425" t="s">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="4426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4426" t="s">
+        <v>4421</v>
+      </c>
+      <c r="B4426" t="s">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="4427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4427" t="s">
+        <v>4422</v>
+      </c>
+      <c r="B4427" t="s">
+        <v>4422</v>
+      </c>
+    </row>
+    <row r="4428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4428" t="s">
+        <v>4423</v>
+      </c>
+      <c r="B4428" t="s">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="4429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4429" t="s">
+        <v>4424</v>
+      </c>
+      <c r="B4429" t="s">
+        <v>4424</v>
+      </c>
+    </row>
+    <row r="4430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4430" t="s">
+        <v>4425</v>
+      </c>
+      <c r="B4430" t="s">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="4431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4431" t="s">
+        <v>4426</v>
+      </c>
+      <c r="B4431" t="s">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="4432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4432" t="s">
+        <v>4427</v>
+      </c>
+      <c r="B4432" t="s">
+        <v>4427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải nghĩa hoàn thiện Ân Quang Thiên Quý 12 cung
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59E1D01-A107-4209-A1AD-682407CE1837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89E9D0F-7582-4F7E-9244-F3005CF056E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8856" uniqueCount="4428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8858" uniqueCount="4430">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13309,6 +13309,12 @@
   </si>
   <si>
     <t>Thất Sát đồng cung Phá Quân tại cung đối Tử Tức</t>
+  </si>
+  <si>
+    <t>Ân Quang Đào Hồng  hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Được cô chú cho đất ở</t>
   </si>
 </sst>
 </file>
@@ -13847,10 +13853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4432"/>
+  <dimension ref="A1:B4433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4317" workbookViewId="0">
-      <selection activeCell="B4342" sqref="B4342:B4432"/>
+    <sheetView tabSelected="1" topLeftCell="A4412" workbookViewId="0">
+      <selection activeCell="E4438" sqref="E4438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49277,6 +49283,14 @@
       </c>
       <c r="B4432" t="s">
         <v>4427</v>
+      </c>
+    </row>
+    <row r="4433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4433" t="s">
+        <v>4428</v>
+      </c>
+      <c r="B4433" t="s">
+        <v>4429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải thichs điền trạch
</commit_message>
<xml_diff>
--- a/LuanDienTrach.xlsx
+++ b/LuanDienTrach.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B0C473-7741-4D75-ABE6-5C62D825A3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21A0C25-5884-45A9-B1FE-712F70E8BCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8926" uniqueCount="4559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8938" uniqueCount="4566">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13709,6 +13709,27 @@
   </si>
   <si>
     <t>Thiên Khốc toạ thủ cung Điền Trạch tại Thìn gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Riêu Hỏa Linh Tấu Thư</t>
+  </si>
+  <si>
+    <t>Riêu Hỏa Linh Tấu Thư hội chiếu Điền Trạch</t>
+  </si>
+  <si>
+    <t>Con ma rất quái ác sẽ bị đánh bật đi.</t>
+  </si>
+  <si>
+    <t>Hỏa Linh Tấu Thư</t>
+  </si>
+  <si>
+    <t>Hỏa Linh Tấu Thư hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cung Điền Trạch an tại Thìn</t>
+  </si>
+  <si>
+    <t>Nếu có ma quỷ quấy nhiễu cũng bị đẩy lui</t>
   </si>
 </sst>
 </file>
@@ -14293,10 +14314,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4466"/>
+  <dimension ref="A1:B4472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4444" workbookViewId="0">
-      <selection activeCell="F4458" sqref="F4458"/>
+    <sheetView tabSelected="1" topLeftCell="A4482" workbookViewId="0">
+      <selection activeCell="E4506" sqref="E4506:F4506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50006,6 +50027,54 @@
       </c>
       <c r="B4466" s="1" t="s">
         <v>4557</v>
+      </c>
+    </row>
+    <row r="4467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4467" s="1" t="s">
+        <v>4559</v>
+      </c>
+      <c r="B4467" s="1" t="s">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="4468" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4468" s="1" t="s">
+        <v>4560</v>
+      </c>
+      <c r="B4468" s="1" t="s">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="4469" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4469" s="1" t="s">
+        <v>4563</v>
+      </c>
+      <c r="B4469" s="1" t="s">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="4470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4470" s="1" t="s">
+        <v>4562</v>
+      </c>
+      <c r="B4470" s="1" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="4471" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4471" s="1" t="s">
+        <v>4564</v>
+      </c>
+      <c r="B4471" s="1" t="s">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="4472" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4472" s="1" t="s">
+        <v>4562</v>
+      </c>
+      <c r="B4472" s="1" t="s">
+        <v>4565</v>
       </c>
     </row>
   </sheetData>
@@ -50032,45 +50101,45 @@
   <conditionalFormatting sqref="A1809:A3338">
     <cfRule type="duplicateValues" dxfId="16" priority="50"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A2602 A2603:B4460 A1:B2601 A4461 A4462:B1048576">
+    <cfRule type="duplicateValues" dxfId="15" priority="4"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A3851:A3912">
-    <cfRule type="duplicateValues" dxfId="15" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2602 A2603:B4460 A1:B2601 A4461 A4462:B1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
+  <conditionalFormatting sqref="B1:B4460 B4462:B1048576">
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B211">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1560">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1804:B1808 B1:B23 B25:B84 B143 B3913:B4211 B6757:B1048576 B3441:B3850 B209:B1631">
-    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1809:B2601 B2603:B3338">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3851:B3912">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4435">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1560">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B4460 B4462:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>